<commit_message>
Added gameboardObject and fixed library dependencies.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prog 4\Stream-Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D645AF-FACB-4BC6-8F60-85C8EDF4E5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8046C6-49B5-42F8-ACC4-43C561A445A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>TO-DO 6/05/2021</t>
   </si>
@@ -88,6 +88,39 @@
   </si>
   <si>
     <t>Optioneel: Teleportation disks</t>
+  </si>
+  <si>
+    <t>Done 20/05/2021</t>
+  </si>
+  <si>
+    <t>TO-DO 27/05/2021</t>
+  </si>
+  <si>
+    <t>Art-work Q*bert</t>
+  </si>
+  <si>
+    <t>Done 27/05/2021</t>
+  </si>
+  <si>
+    <t>TO-DO 3/06/2021</t>
+  </si>
+  <si>
+    <t>Done 3/06/2021</t>
+  </si>
+  <si>
+    <t>TO-DO Final 7/06/2021</t>
+  </si>
+  <si>
+    <t>Game-board Implementeren 4 slots</t>
+  </si>
+  <si>
+    <t>Teleportation disks 2 slots</t>
+  </si>
+  <si>
+    <t>Coily enemy char 4 slots</t>
+  </si>
+  <si>
+    <t>Point system 2 slots</t>
   </si>
 </sst>
 </file>
@@ -406,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,9 +452,15 @@
     <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="53.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44315</v>
       </c>
@@ -440,8 +479,26 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -460,8 +517,14 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -477,8 +540,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -494,8 +560,11 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -508,16 +577,22 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>14</v>
       </c>

</xml_diff>